<commit_message>
New updates in some column names
Former-commit-id: 8d764fcb41c8477ffbcd13e2a6fd485e8917fa7b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>[sku]</t>
   </si>
@@ -65,21 +65,12 @@
     <t>xPromoSettings</t>
   </si>
   <si>
-    <t>{localRewardsDefinitions}</t>
-  </si>
-  <si>
-    <t>[game]</t>
-  </si>
-  <si>
     <t>[day]</t>
   </si>
   <si>
     <t>[rewardSku]</t>
   </si>
   <si>
-    <t>[priority]</t>
-  </si>
-  <si>
     <t>reward_2</t>
   </si>
   <si>
@@ -116,15 +107,9 @@
     <t>pet_67</t>
   </si>
   <si>
-    <t>[group]</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>[recruitingDuration]</t>
-  </si>
-  <si>
     <t>recruitingDuration: Days when players can start the xpromo, starting from [startDate]</t>
   </si>
   <si>
@@ -137,18 +122,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>[typeAlt]</t>
-  </si>
-  <si>
-    <t>[amountAlt]</t>
-  </si>
-  <si>
-    <t>Coins</t>
-  </si>
-  <si>
-    <t>Gems</t>
-  </si>
-  <si>
     <t>coins</t>
   </si>
   <si>
@@ -174,6 +147,27 @@
   </si>
   <si>
     <t>TID_blablablabla</t>
+  </si>
+  <si>
+    <t>[recruitingLimitDate]</t>
+  </si>
+  <si>
+    <t>[ABgroup]</t>
+  </si>
+  <si>
+    <t>{xPromoRewardsDefinitions}</t>
+  </si>
+  <si>
+    <t>[destination]</t>
+  </si>
+  <si>
+    <t>[origin]</t>
+  </si>
+  <si>
+    <t>[altSC]</t>
+  </si>
+  <si>
+    <t>[altPC]</t>
   </si>
 </sst>
 </file>
@@ -627,6 +621,46 @@
         <left style="thin">
           <color auto="1"/>
         </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
         <right/>
         <top style="thin">
           <color auto="1"/>
@@ -1021,44 +1055,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1501,38 +1497,38 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table52" displayName="Table52" ref="A11:N15" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A11:N15"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="{localRewardsDefinitions}" dataDxfId="28"/>
+    <tableColumn id="1" name="{xPromoRewardsDefinitions}" dataDxfId="28"/>
     <tableColumn id="2" name="[sku]" dataDxfId="27"/>
     <tableColumn id="3" name="[enabled]" dataDxfId="26"/>
-    <tableColumn id="13" name="[group]" dataDxfId="4"/>
+    <tableColumn id="13" name="[ABgroup]" dataDxfId="5"/>
     <tableColumn id="4" name="[day]" dataDxfId="25"/>
-    <tableColumn id="5" name="[game]" dataDxfId="3"/>
+    <tableColumn id="16" name="[origin]" dataDxfId="1"/>
+    <tableColumn id="5" name="[destination]" dataDxfId="4"/>
     <tableColumn id="6" name="[type]" dataDxfId="24"/>
     <tableColumn id="7" name="[amount]" dataDxfId="23"/>
     <tableColumn id="8" name="[rewardSku]" dataDxfId="22"/>
-    <tableColumn id="14" name="[typeAlt]" dataDxfId="2"/>
-    <tableColumn id="15" name="[amountAlt]" dataDxfId="1"/>
+    <tableColumn id="14" name="[altSC]" dataDxfId="3"/>
+    <tableColumn id="15" name="[altPC]" dataDxfId="2"/>
     <tableColumn id="9" name="[icon]" dataDxfId="21"/>
     <tableColumn id="10" name="[tid]" dataDxfId="20"/>
-    <tableColumn id="11" name="[priority]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
   <autoFilter ref="A3:I4"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="{xPromoSettings}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="11"/>
-    <tableColumn id="8" name="[group]" dataDxfId="10"/>
-    <tableColumn id="4" name="[startDate]" dataDxfId="9"/>
-    <tableColumn id="5" name="[endDate]" dataDxfId="8"/>
-    <tableColumn id="10" name="[recruitingDuration]" dataDxfId="7"/>
-    <tableColumn id="6" name="[minRuns]" dataDxfId="6"/>
-    <tableColumn id="7" name="[cycleSize]" dataDxfId="5"/>
+    <tableColumn id="1" name="{xPromoSettings}" dataDxfId="14"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="12"/>
+    <tableColumn id="8" name="[ABgroup]" dataDxfId="11"/>
+    <tableColumn id="4" name="[startDate]" dataDxfId="10"/>
+    <tableColumn id="5" name="[endDate]" dataDxfId="9"/>
+    <tableColumn id="10" name="[recruitingLimitDate]" dataDxfId="8"/>
+    <tableColumn id="6" name="[minRuns]" dataDxfId="7"/>
+    <tableColumn id="7" name="[cycleSize]" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1807,7 +1803,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,6 +1820,7 @@
     <col min="10" max="10" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="27" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
@@ -1844,7 +1841,7 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="102" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="105.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1855,7 +1852,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -1864,7 +1861,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
@@ -1884,7 +1881,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E4" s="15">
         <v>0</v>
@@ -1904,18 +1901,18 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1931,9 +1928,9 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:14" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
@@ -1942,37 +1939,37 @@
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="K11" s="13" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="L11" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="M11" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="N11" s="13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1980,43 +1977,41 @@
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C12" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>21</v>
+      <c r="F12" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="9">
+        <v>18</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="9">
         <v>1</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="J12" s="11" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="K12" s="11">
         <v>5000</v>
       </c>
-      <c r="L12" s="11" t="s">
-        <v>46</v>
-      </c>
+      <c r="L12" s="11"/>
       <c r="M12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="N12" s="11">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2024,37 +2019,37 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C13" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>22</v>
+      <c r="F13" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="9">
+        <v>19</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="9">
         <v>7000</v>
       </c>
-      <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="L13" s="10"/>
       <c r="M13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" s="10">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2062,43 +2057,41 @@
         <v>1</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E14" s="10">
         <v>1</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="9">
+      <c r="I14" s="9">
         <v>1</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="J14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10">
+        <v>20</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N14" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="K14" s="10">
-        <v>20</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="N14" s="10">
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2106,43 +2099,41 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E15" s="12">
         <v>2</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>22</v>
+      <c r="F15" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="9">
+        <v>19</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="9">
         <v>1</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="J15" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="12">
+        <v>34</v>
+      </c>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12">
         <v>20</v>
       </c>
-      <c r="L15" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="M15" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="12">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xPromo - Add content to the excel table
Former-commit-id: 028af70894c992b6d4de29e47536958b1887d782
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68413972-03CF-1141-A3B8-7DF51DFFB2C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="19500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Special Leagues" sheetId="16" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
   <si>
     <t>[sku]</t>
   </si>
@@ -71,15 +72,6 @@
     <t>[rewardSku]</t>
   </si>
   <si>
-    <t>reward_2</t>
-  </si>
-  <si>
-    <t>reward_3</t>
-  </si>
-  <si>
-    <t>reward_4</t>
-  </si>
-  <si>
     <t>hd</t>
   </si>
   <si>
@@ -116,9 +108,6 @@
     <t>REWARDS</t>
   </si>
   <si>
-    <t>reward_1</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -128,27 +117,15 @@
     <t>shark</t>
   </si>
   <si>
-    <t>shark_white</t>
-  </si>
-  <si>
     <t>group: needed only for AB test. Json for group A should set this variable ="A", and json for group B should set this variable ="B"</t>
   </si>
   <si>
     <t>xpromo_hse_coins</t>
   </si>
   <si>
-    <t>xpromo_hd_coins</t>
-  </si>
-  <si>
     <t>xpromo_hse_shark_white</t>
   </si>
   <si>
-    <t>xpromo_hd_dragon_chinese</t>
-  </si>
-  <si>
-    <t>TID_blablablabla</t>
-  </si>
-  <si>
     <t>[recruitingLimitDate]</t>
   </si>
   <si>
@@ -168,12 +145,69 @@
   </si>
   <si>
     <t>[altPC]</t>
+  </si>
+  <si>
+    <t>12/31/2020  00:00:00</t>
+  </si>
+  <si>
+    <t>Field to be filled by HSE designers</t>
+  </si>
+  <si>
+    <t>reward_hd_1a</t>
+  </si>
+  <si>
+    <t>reward_hd_2a</t>
+  </si>
+  <si>
+    <t>reward_hd_3a</t>
+  </si>
+  <si>
+    <t>reward_hd_4a</t>
+  </si>
+  <si>
+    <t>reward_hd_5a</t>
+  </si>
+  <si>
+    <t>reward_hd_1b</t>
+  </si>
+  <si>
+    <t>reward_hd_2b</t>
+  </si>
+  <si>
+    <t>reward_hd_3b</t>
+  </si>
+  <si>
+    <t>reward_hd_4b</t>
+  </si>
+  <si>
+    <t>reward_hd_5b</t>
+  </si>
+  <si>
+    <t>reward_hse_1a</t>
+  </si>
+  <si>
+    <t>pet_59</t>
+  </si>
+  <si>
+    <t>reward_hse_3a</t>
+  </si>
+  <si>
+    <t>reward_hse_2a</t>
+  </si>
+  <si>
+    <t>dragon_umbra</t>
+  </si>
+  <si>
+    <t>reward_hse_4a</t>
+  </si>
+  <si>
+    <t>mega_tuna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,8 +285,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -335,19 +381,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -373,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -385,9 +418,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -395,35 +425,210 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -456,22 +661,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -496,22 +705,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -539,19 +752,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -579,19 +796,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -616,22 +837,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -656,18 +881,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -692,20 +925,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -733,17 +972,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -771,17 +1016,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -806,20 +1057,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -847,17 +1104,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -882,20 +1145,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -920,20 +1189,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -958,45 +1233,26 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
-          <color auto="1"/>
+          <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1015,6 +1271,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1022,6 +1279,372 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1055,344 +1678,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1494,41 +1779,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table52" displayName="Table52" ref="A11:N15" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
-  <autoFilter ref="A11:N15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table52" displayName="Table52" ref="A11:N16" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+  <autoFilter ref="A11:N16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="{xPromoRewardsDefinitions}" dataDxfId="28"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="27"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="26"/>
-    <tableColumn id="13" name="[ABgroup]" dataDxfId="5"/>
-    <tableColumn id="4" name="[day]" dataDxfId="25"/>
-    <tableColumn id="16" name="[origin]" dataDxfId="1"/>
-    <tableColumn id="5" name="[destination]" dataDxfId="4"/>
-    <tableColumn id="6" name="[type]" dataDxfId="24"/>
-    <tableColumn id="7" name="[amount]" dataDxfId="23"/>
-    <tableColumn id="8" name="[rewardSku]" dataDxfId="22"/>
-    <tableColumn id="14" name="[altSC]" dataDxfId="3"/>
-    <tableColumn id="15" name="[altPC]" dataDxfId="2"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="21"/>
-    <tableColumn id="10" name="[tid]" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{xPromoRewardsDefinitions}" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="28"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[ABgroup]" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[day]" dataDxfId="26"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[origin]" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[destination]" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[type]" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[amount]" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[rewardSku]" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[altSC]" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[altPC]" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[icon]" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tid]" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
-  <autoFilter ref="A3:I4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+  <autoFilter ref="A3:I4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="{xPromoSettings}" dataDxfId="14"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="12"/>
-    <tableColumn id="8" name="[ABgroup]" dataDxfId="11"/>
-    <tableColumn id="4" name="[startDate]" dataDxfId="10"/>
-    <tableColumn id="5" name="[endDate]" dataDxfId="9"/>
-    <tableColumn id="10" name="[recruitingLimitDate]" dataDxfId="8"/>
-    <tableColumn id="6" name="[minRuns]" dataDxfId="7"/>
-    <tableColumn id="7" name="[cycleSize]" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{xPromoSettings}" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[enabled]" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[ABgroup]" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[startDate]" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[endDate]" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[recruitingLimitDate]" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[minRuns]" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[cycleSize]" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1796,34 +2081,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
     <col min="12" max="12" width="27" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1835,13 +2120,13 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="105.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="103" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1852,7 +2137,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -1861,58 +2146,58 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="15" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="15">
-        <v>0</v>
-      </c>
-      <c r="F4" s="15">
-        <v>0</v>
-      </c>
-      <c r="G4" s="15">
+      <c r="C4" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="13">
+        <v>43831</v>
+      </c>
+      <c r="F4" s="13">
+        <v>43842</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="11">
+        <v>3</v>
+      </c>
+      <c r="I4" s="12">
         <v>5</v>
       </c>
-      <c r="H4" s="15">
-        <v>3</v>
-      </c>
-      <c r="I4" s="16">
-        <v>2</v>
-      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:14" ht="24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1922,15 +2207,15 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:14" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="137" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
@@ -1939,206 +2224,609 @@
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1000</v>
+      </c>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="8">
+        <v>3</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="6">
+        <v>7000</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="8">
+        <v>5</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="8">
+        <v>5000</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="8">
+        <v>7</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="C16" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="6">
+        <v>9</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6">
+        <v>5</v>
+      </c>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="M11" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="13" t="s">
+      <c r="C17" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="6">
+        <v>1</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1000</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="8">
+        <v>3</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="6">
+        <v>7000</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="8">
+        <v>5</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="K19" s="8">
+        <v>5000</v>
+      </c>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="11">
-        <v>1</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="E20" s="8">
+        <v>7</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="21">
+        <v>9</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="I21" s="21">
+        <v>1</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21">
+        <v>5</v>
+      </c>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+    </row>
+    <row r="22" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="15">
+        <v>1</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="15">
+        <v>3</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="15">
+        <v>1</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="15">
+        <v>1000</v>
+      </c>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="15">
+        <v>5</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="15">
+        <v>7</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="I25" s="15">
+        <v>1</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15">
         <v>20</v>
       </c>
-      <c r="I12" s="9">
-        <v>1</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="11">
-        <v>5000</v>
-      </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="N12" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="10">
-        <v>2</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="9">
-        <v>7000</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="10">
-        <v>1</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="9">
-        <v>1</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10">
-        <v>20</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="12">
-        <v>2</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="9">
-        <v>1</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12">
-        <v>20</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="N15" s="12" t="s">
-        <v>24</v>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B12:B15">
-    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  <conditionalFormatting sqref="B12:B16">
+    <cfRule type="duplicateValues" dxfId="16" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21">
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
xPromo - Fix bugs in excel doc
Former-commit-id: 2731d98e84635973219ccc9e3552891d78260082
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68413972-03CF-1141-A3B8-7DF51DFFB2C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65745DA-B1A8-4541-B3E3-523007CAA151}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
   <si>
     <t>[sku]</t>
   </si>
@@ -120,18 +120,9 @@
     <t>group: needed only for AB test. Json for group A should set this variable ="A", and json for group B should set this variable ="B"</t>
   </si>
   <si>
-    <t>xpromo_hse_coins</t>
-  </si>
-  <si>
-    <t>xpromo_hse_shark_white</t>
-  </si>
-  <si>
     <t>[recruitingLimitDate]</t>
   </si>
   <si>
-    <t>[ABgroup]</t>
-  </si>
-  <si>
     <t>{xPromoRewardsDefinitions}</t>
   </si>
   <si>
@@ -147,9 +138,6 @@
     <t>[altPC]</t>
   </si>
   <si>
-    <t>12/31/2020  00:00:00</t>
-  </si>
-  <si>
     <t>Field to be filled by HSE designers</t>
   </si>
   <si>
@@ -201,7 +189,28 @@
     <t>reward_hse_4a</t>
   </si>
   <si>
-    <t>mega_tuna</t>
+    <t>12/31/2020 00:00:00</t>
+  </si>
+  <si>
+    <t>01/01/2020 00:00:00</t>
+  </si>
+  <si>
+    <t>12/01/2020 00:00:00</t>
+  </si>
+  <si>
+    <t>[ABGroup]</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>SD_shark_moby</t>
+  </si>
+  <si>
+    <t>SD_shark_hammerhead</t>
+  </si>
+  <si>
+    <t>egg_babyGuaranteed</t>
   </si>
 </sst>
 </file>
@@ -440,9 +449,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -464,181 +470,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="50">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -655,32 +494,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -699,32 +533,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -743,6 +572,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -752,24 +582,188 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -793,7 +787,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -881,7 +875,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -925,7 +919,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -969,7 +963,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1013,7 +1007,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1145,7 +1139,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1213,6 +1207,138 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1253,122 +1379,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1782,20 +1792,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table52" displayName="Table52" ref="A11:N16" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="A11:N16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{xPromoRewardsDefinitions}" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="28"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[ABgroup]" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[day]" dataDxfId="26"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[origin]" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[destination]" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[type]" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[amount]" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[rewardSku]" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[altSC]" dataDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[altPC]" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[icon]" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tid]" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{xPromoRewardsDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[ABGroup]" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[day]" dataDxfId="29"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[origin]" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[destination]" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[type]" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[amount]" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[rewardSku]" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[altSC]" dataDxfId="23"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[altPC]" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[icon]" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tid]" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1808,10 +1818,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{xPromoSettings}" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="38"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[enabled]" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[ABgroup]" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[startDate]" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[endDate]" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[recruitingLimitDate]" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[ABGroup]" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[startDate]" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[endDate]" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[recruitingLimitDate]" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[minRuns]" dataDxfId="35"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[cycleSize]" dataDxfId="34"/>
   </tableColumns>
@@ -2087,8 +2097,8 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2105,7 +2115,7 @@
     <col min="10" max="10" width="20.5" customWidth="1"/>
     <col min="12" max="12" width="27" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
@@ -2137,7 +2147,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -2146,7 +2156,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
@@ -2168,14 +2178,14 @@
       <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="13">
-        <v>43831</v>
-      </c>
-      <c r="F4" s="13">
-        <v>43842</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>40</v>
+      <c r="E4" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>54</v>
       </c>
       <c r="H4" s="11">
         <v>3</v>
@@ -2215,7 +2225,7 @@
     </row>
     <row r="11" spans="1:14" ht="137" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
@@ -2224,16 +2234,16 @@
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>3</v>
@@ -2245,10 +2255,10 @@
         <v>14</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M11" s="9" t="s">
         <v>2</v>
@@ -2258,11 +2268,11 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="b">
         <v>1</v>
@@ -2296,11 +2306,11 @@
       <c r="N12" s="8"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" s="6" t="b">
         <v>1</v>
@@ -2320,25 +2330,23 @@
       <c r="H13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="6">
-        <v>7000</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="8" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="b">
         <v>1</v>
@@ -2372,11 +2380,11 @@
       <c r="N14" s="8"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="b">
         <v>1</v>
@@ -2396,27 +2404,23 @@
       <c r="H15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="6">
-        <v>1</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
       <c r="M15" s="8" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C16" s="6" t="b">
         <v>1</v>
@@ -2434,13 +2438,13 @@
         <v>15</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="I16" s="6">
         <v>1</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>22</v>
+      <c r="J16" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6">
@@ -2450,11 +2454,11 @@
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" s="6" t="b">
         <v>1</v>
@@ -2477,22 +2481,22 @@
       <c r="I17" s="6">
         <v>1</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K17" s="8">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C18" s="6" t="b">
         <v>1</v>
@@ -2512,25 +2516,23 @@
       <c r="H18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="6">
-        <v>7000</v>
-      </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="8" t="s">
-        <v>31</v>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="N18" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C19" s="6" t="b">
         <v>1</v>
@@ -2564,11 +2566,11 @@
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C20" s="6" t="b">
         <v>1</v>
@@ -2588,247 +2590,244 @@
       <c r="H20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="6">
-        <v>1</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="8" t="s">
-        <v>32</v>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="N20" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="22" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" s="21" t="s">
+    <row r="21" spans="1:14" s="21" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="20">
         <v>9</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F21" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="21">
-        <v>1</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21">
+      <c r="I21" s="20">
+        <v>1</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20">
         <v>5</v>
       </c>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" s="15" t="s">
+      <c r="A22" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="15">
-        <v>1</v>
-      </c>
-      <c r="F22" s="15" t="s">
+      <c r="E22" s="14">
+        <v>1</v>
+      </c>
+      <c r="F22" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
     </row>
-    <row r="23" spans="1:14" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="15" t="s">
+    <row r="23" spans="1:14" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="14">
         <v>3</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="15">
-        <v>1</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="K23" s="15">
+      <c r="I23" s="14">
+        <v>1</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K23" s="14">
         <v>1000</v>
       </c>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
     </row>
     <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="15" t="s">
+      <c r="A24" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="14">
         <v>5</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
     </row>
-    <row r="25" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="15" t="s">
+    <row r="25" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="14">
         <v>7</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="15">
-        <v>1</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15">
+      <c r="I25" s="14">
+        <v>1</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14">
         <v>20</v>
       </c>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>41</v>
+      <c r="A27" s="15" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="duplicateValues" dxfId="16" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
xPromo - Fix incoming reward system. Fix content with new skus.
Former-commit-id: 67f99ab9aa74fde9bc53a493828006f8eff64a97
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65745DA-B1A8-4541-B3E3-523007CAA151}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99C04D1-E514-AD4A-B0B2-6D2360189017}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="66">
   <si>
     <t>[sku]</t>
   </si>
@@ -141,54 +141,9 @@
     <t>Field to be filled by HSE designers</t>
   </si>
   <si>
-    <t>reward_hd_1a</t>
-  </si>
-  <si>
-    <t>reward_hd_2a</t>
-  </si>
-  <si>
-    <t>reward_hd_3a</t>
-  </si>
-  <si>
-    <t>reward_hd_4a</t>
-  </si>
-  <si>
-    <t>reward_hd_5a</t>
-  </si>
-  <si>
-    <t>reward_hd_1b</t>
-  </si>
-  <si>
-    <t>reward_hd_2b</t>
-  </si>
-  <si>
-    <t>reward_hd_3b</t>
-  </si>
-  <si>
-    <t>reward_hd_4b</t>
-  </si>
-  <si>
-    <t>reward_hd_5b</t>
-  </si>
-  <si>
-    <t>reward_hse_1a</t>
-  </si>
-  <si>
-    <t>pet_59</t>
-  </si>
-  <si>
-    <t>reward_hse_3a</t>
-  </si>
-  <si>
-    <t>reward_hse_2a</t>
-  </si>
-  <si>
     <t>dragon_umbra</t>
   </si>
   <si>
-    <t>reward_hse_4a</t>
-  </si>
-  <si>
     <t>12/31/2020 00:00:00</t>
   </si>
   <si>
@@ -211,6 +166,63 @@
   </si>
   <si>
     <t>egg_babyGuaranteed</t>
+  </si>
+  <si>
+    <t>[experiment]</t>
+  </si>
+  <si>
+    <t>reward_hd_hse_1a</t>
+  </si>
+  <si>
+    <t>reward_hd_hse_1b</t>
+  </si>
+  <si>
+    <t>reward_hd_hse_2b</t>
+  </si>
+  <si>
+    <t>reward_hse_hd_2a</t>
+  </si>
+  <si>
+    <t>reward_hse_hd_1a</t>
+  </si>
+  <si>
+    <t>reward_hd_hd_1a</t>
+  </si>
+  <si>
+    <t>reward_hd_hd_2a</t>
+  </si>
+  <si>
+    <t>reward_hd_hd_3a</t>
+  </si>
+  <si>
+    <t>reward_hd_hd_1b</t>
+  </si>
+  <si>
+    <t>reward_hd_hd_2b</t>
+  </si>
+  <si>
+    <t>reward_hd_hd_3b</t>
+  </si>
+  <si>
+    <t>reward_hd_hse_2a</t>
+  </si>
+  <si>
+    <t>reward_hse_hse_1a</t>
+  </si>
+  <si>
+    <t>reward_hse_hse_2a</t>
+  </si>
+  <si>
+    <t>egg_betterRates</t>
+  </si>
+  <si>
+    <t>pet_33</t>
+  </si>
+  <si>
+    <t>reward_hse_hd_3a</t>
+  </si>
+  <si>
+    <t>dragon_reptile</t>
   </si>
 </sst>
 </file>
@@ -260,12 +272,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -307,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -411,11 +425,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -473,11 +498,34 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -533,7 +581,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -545,9 +592,7 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -572,7 +617,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -594,176 +638,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -781,32 +655,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -825,32 +694,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -869,6 +733,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -878,23 +743,17 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -922,23 +781,17 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -963,26 +816,20 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1007,26 +854,76 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1051,26 +948,47 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1095,7 +1013,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1139,7 +1057,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1183,7 +1101,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1339,6 +1257,314 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1382,6 +1608,26 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1403,251 +1649,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1691,89 +1693,154 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1789,41 +1856,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table52" displayName="Table52" ref="A11:N16" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table52" displayName="Table52" ref="A11:N16" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="A11:N16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{xPromoRewardsDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[ABGroup]" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[day]" dataDxfId="29"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[origin]" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[destination]" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[type]" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[amount]" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[rewardSku]" dataDxfId="24"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[altSC]" dataDxfId="23"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[altPC]" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[icon]" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tid]" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{xPromoRewardsDefinitions}" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="28"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[ABGroup]" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[day]" dataDxfId="26"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[origin]" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[destination]" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[type]" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[amount]" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[rewardSku]" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[altSC]" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[altPC]" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[icon]" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tid]" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
-  <autoFilter ref="A3:I4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{xPromoSettings}" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[enabled]" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[ABGroup]" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[startDate]" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[endDate]" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[recruitingLimitDate]" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[minRuns]" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[cycleSize]" dataDxfId="34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A3:J4" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A3:J4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{xPromoSettings}" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[enabled]" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[ABGroup]" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[startDate]" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[endDate]" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[recruitingLimitDate]" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[minRuns]" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[cycleSize]" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{D7916C4D-35E2-864E-86A1-D933FAC4245A}" name="[experiment]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2097,8 +2165,8 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2147,7 +2215,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -2163,6 +2231,9 @@
       </c>
       <c r="I3" s="7" t="s">
         <v>11</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2179,13 +2250,13 @@
         <v>24</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="H4" s="11">
         <v>3</v>
@@ -2193,6 +2264,7 @@
       <c r="I4" s="12">
         <v>5</v>
       </c>
+      <c r="J4" s="23"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2234,7 +2306,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -2272,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="b">
         <v>1</v>
@@ -2310,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C13" s="6" t="b">
         <v>1</v>
@@ -2335,7 +2407,7 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="8" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>20</v>
@@ -2346,7 +2418,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C14" s="6" t="b">
         <v>1</v>
@@ -2384,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C15" s="6" t="b">
         <v>1</v>
@@ -2409,7 +2481,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>21</v>
@@ -2420,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6" t="b">
         <v>1</v>
@@ -2438,13 +2510,13 @@
         <v>15</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="I16" s="6">
         <v>1</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6">
@@ -2458,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6" t="b">
         <v>1</v>
@@ -2496,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C18" s="6" t="b">
         <v>1</v>
@@ -2521,7 +2593,7 @@
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="6" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="N18" s="8" t="s">
         <v>20</v>
@@ -2532,7 +2604,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C19" s="6" t="b">
         <v>1</v>
@@ -2570,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C20" s="6" t="b">
         <v>1</v>
@@ -2595,7 +2667,7 @@
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="6" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="N20" s="8" t="s">
         <v>21</v>
@@ -2606,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C21" s="20" t="b">
         <v>1</v>
@@ -2630,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20">
@@ -2644,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C22" s="14" t="b">
         <v>1</v>
@@ -2674,7 +2746,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="14" t="b">
         <v>1</v>
@@ -2692,13 +2764,13 @@
         <v>15</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="I23" s="14">
         <v>1</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="K23" s="14">
         <v>1000</v>
@@ -2712,7 +2784,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C24" s="14" t="b">
         <v>1</v>
@@ -2742,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="14" t="b">
         <v>1</v>
@@ -2760,20 +2832,58 @@
         <v>15</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I25" s="14">
         <v>1</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14">
-        <v>20</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="K25" s="14">
+        <v>20000</v>
+      </c>
+      <c r="L25" s="14"/>
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
+    </row>
+    <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="14">
+        <v>5</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="14">
+        <v>1</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14">
+        <v>20</v>
+      </c>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
@@ -2782,49 +2892,55 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="duplicateValues" dxfId="19" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="16" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="14" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
xPromo - Fix grey tick y xpromo popup. Change date format to timestamp in content.
Former-commit-id: 9fec40a3019b7d40ba7ec30ee5b7488b6cffe445
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99C04D1-E514-AD4A-B0B2-6D2360189017}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594AA644-AA1B-3B40-9549-AAA7C5593F7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,15 +144,6 @@
     <t>dragon_umbra</t>
   </si>
   <si>
-    <t>12/31/2020 00:00:00</t>
-  </si>
-  <si>
-    <t>01/01/2020 00:00:00</t>
-  </si>
-  <si>
-    <t>12/01/2020 00:00:00</t>
-  </si>
-  <si>
     <t>[ABGroup]</t>
   </si>
   <si>
@@ -223,6 +214,15 @@
   </si>
   <si>
     <t>dragon_reptile</t>
+  </si>
+  <si>
+    <t>1577836800</t>
+  </si>
+  <si>
+    <t>1609372800</t>
+  </si>
+  <si>
+    <t>1606780800</t>
   </si>
 </sst>
 </file>
@@ -508,26 +508,6 @@
   <dxfs count="51">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -567,6 +547,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -581,6 +581,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -592,7 +593,9 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -628,9 +631,7 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -655,7 +656,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1887,11 +1887,11 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[enabled]" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[ABGroup]" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[startDate]" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[endDate]" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[recruitingLimitDate]" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[minRuns]" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[cycleSize]" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{D7916C4D-35E2-864E-86A1-D933FAC4245A}" name="[experiment]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[endDate]" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[recruitingLimitDate]" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[minRuns]" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[cycleSize]" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{D7916C4D-35E2-864E-86A1-D933FAC4245A}" name="[experiment]" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2165,8 +2165,8 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2215,7 +2215,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -2233,7 +2233,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2250,13 +2250,13 @@
         <v>24</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="H4" s="11">
         <v>3</v>
@@ -2306,7 +2306,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C12" s="6" t="b">
         <v>1</v>
@@ -2382,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13" s="6" t="b">
         <v>1</v>
@@ -2407,7 +2407,7 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>20</v>
@@ -2418,7 +2418,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" s="6" t="b">
         <v>1</v>
@@ -2456,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" s="6" t="b">
         <v>1</v>
@@ -2481,7 +2481,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>21</v>
@@ -2492,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C16" s="6" t="b">
         <v>1</v>
@@ -2510,13 +2510,13 @@
         <v>15</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="I16" s="6">
-        <v>1</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6">
@@ -2530,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C17" s="6" t="b">
         <v>1</v>
@@ -2568,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C18" s="6" t="b">
         <v>1</v>
@@ -2593,7 +2593,7 @@
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N18" s="8" t="s">
         <v>20</v>
@@ -2604,7 +2604,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6" t="b">
         <v>1</v>
@@ -2642,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C20" s="6" t="b">
         <v>1</v>
@@ -2667,7 +2667,7 @@
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N20" s="8" t="s">
         <v>21</v>
@@ -2678,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21" s="20" t="b">
         <v>1</v>
@@ -2716,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C22" s="14" t="b">
         <v>1</v>
@@ -2746,7 +2746,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C23" s="14" t="b">
         <v>1</v>
@@ -2764,13 +2764,13 @@
         <v>15</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I23" s="14">
         <v>1</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K23" s="14">
         <v>1000</v>
@@ -2784,7 +2784,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C24" s="14" t="b">
         <v>1</v>
@@ -2814,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C25" s="14" t="b">
         <v>1</v>
@@ -2838,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K25" s="14">
         <v>20000</v>
@@ -2852,7 +2852,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C26" s="14" t="b">
         <v>1</v>
@@ -2876,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K26" s="14"/>
       <c r="L26" s="14">
@@ -2937,10 +2937,10 @@
     <cfRule type="duplicateValues" dxfId="36" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated for ab test duration 3 days
Former-commit-id: eaad69065303437e2f8847078d22cdaf9a9ad456
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="19200" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="Special Leagues" sheetId="16" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
   <si>
     <t>[sku]</t>
   </si>
@@ -92,12 +92,6 @@
     <t>TID_MEGA_TUNA</t>
   </si>
   <si>
-    <t>dragon_chinese</t>
-  </si>
-  <si>
-    <t>pet_67</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>shark</t>
   </si>
   <si>
-    <t>group: needed only for AB test. Json for group A should set this variable ="A", and json for group B should set this variable ="B"</t>
-  </si>
-  <si>
     <t>[recruitingLimitDate]</t>
   </si>
   <si>
@@ -134,12 +125,6 @@
     <t>[altPC]</t>
   </si>
   <si>
-    <t>Field to be filled by HSE designers</t>
-  </si>
-  <si>
-    <t>dragon_umbra</t>
-  </si>
-  <si>
     <t>[ABGroup]</t>
   </si>
   <si>
@@ -152,9 +137,6 @@
     <t>SD_shark_hammerhead</t>
   </si>
   <si>
-    <t>egg_babyGuaranteed</t>
-  </si>
-  <si>
     <t>[experiment]</t>
   </si>
   <si>
@@ -173,33 +155,9 @@
     <t>reward_hse_hd_1a</t>
   </si>
   <si>
-    <t>reward_hd_hd_1a</t>
-  </si>
-  <si>
-    <t>reward_hd_hd_2a</t>
-  </si>
-  <si>
-    <t>reward_hd_hd_3a</t>
-  </si>
-  <si>
-    <t>reward_hd_hd_1b</t>
-  </si>
-  <si>
-    <t>reward_hd_hd_2b</t>
-  </si>
-  <si>
-    <t>reward_hd_hd_3b</t>
-  </si>
-  <si>
     <t>reward_hd_hse_2a</t>
   </si>
   <si>
-    <t>reward_hse_hse_1a</t>
-  </si>
-  <si>
-    <t>reward_hse_hse_2a</t>
-  </si>
-  <si>
     <t>egg_betterRates</t>
   </si>
   <si>
@@ -215,10 +173,46 @@
     <t>recruitingDuration: Days when players can start the xpromo, starting from [startDate] (this is a date also)</t>
   </si>
   <si>
-    <t>1600684515</t>
-  </si>
-  <si>
     <t>cycleSize: How many days player can get a reward (make sure in rewards table we have just those number of rewards defined)</t>
+  </si>
+  <si>
+    <t>1601510400</t>
+  </si>
+  <si>
+    <t>1604102400</t>
+  </si>
+  <si>
+    <t>1602720000</t>
+  </si>
+  <si>
+    <t>group: needed only for AB test. Json for group A should set this variable ="A", and json for group B should set this variable ="B" (so client, reading this, knows in which group is each player)</t>
+  </si>
+  <si>
+    <t>hammerhead</t>
+  </si>
+  <si>
+    <t>accessory</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>moby</t>
+  </si>
+  <si>
+    <t>reward_hd_hse_3a</t>
+  </si>
+  <si>
+    <t>reward_hd_hse_3b</t>
+  </si>
+  <si>
+    <t>gems</t>
+  </si>
+  <si>
+    <t>01-10-2020_test_x_promo_A</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -292,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,20 +311,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -445,11 +427,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -483,21 +495,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -510,11 +511,62 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1235,166 +1287,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1875,42 +1767,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table52" displayName="Table52" ref="A12:N27" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
-  <autoFilter ref="A12:N27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table52" displayName="Table52" ref="A12:N24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+  <autoFilter ref="A12:N24"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="{xPromoRewardsDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="13"/>
-    <tableColumn id="13" name="[ABGroup]" dataDxfId="12"/>
-    <tableColumn id="4" name="[day]" dataDxfId="11"/>
-    <tableColumn id="16" name="[origin]" dataDxfId="10"/>
-    <tableColumn id="5" name="[destination]" dataDxfId="9"/>
-    <tableColumn id="6" name="[type]" dataDxfId="8"/>
-    <tableColumn id="7" name="[amount]" dataDxfId="7"/>
-    <tableColumn id="8" name="[rewardSku]" dataDxfId="6"/>
-    <tableColumn id="14" name="[altSC]" dataDxfId="5"/>
-    <tableColumn id="15" name="[altPC]" dataDxfId="4"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="10" name="[tid]" dataDxfId="2"/>
+    <tableColumn id="1" name="{xPromoRewardsDefinitions}" dataDxfId="18"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="16"/>
+    <tableColumn id="13" name="[ABGroup]" dataDxfId="15"/>
+    <tableColumn id="4" name="[day]" dataDxfId="14"/>
+    <tableColumn id="16" name="[origin]" dataDxfId="13"/>
+    <tableColumn id="5" name="[destination]" dataDxfId="12"/>
+    <tableColumn id="6" name="[type]" dataDxfId="11"/>
+    <tableColumn id="7" name="[amount]" dataDxfId="10"/>
+    <tableColumn id="8" name="[rewardSku]" dataDxfId="9"/>
+    <tableColumn id="14" name="[altSC]" dataDxfId="8"/>
+    <tableColumn id="15" name="[altPC]" dataDxfId="7"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="6"/>
+    <tableColumn id="10" name="[tid]" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:J4" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:J4" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="A3:J4"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{xPromoSettings}" dataDxfId="46"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="45"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="44"/>
-    <tableColumn id="8" name="[ABGroup]" dataDxfId="43"/>
-    <tableColumn id="4" name="[startDate]" dataDxfId="42"/>
-    <tableColumn id="5" name="[endDate]" dataDxfId="41"/>
-    <tableColumn id="10" name="[recruitingLimitDate]" dataDxfId="40"/>
-    <tableColumn id="6" name="[minRuns]" dataDxfId="39"/>
-    <tableColumn id="7" name="[cycleSize]" dataDxfId="38"/>
-    <tableColumn id="9" name="[experiment]" dataDxfId="37"/>
+    <tableColumn id="1" name="{xPromoSettings}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="31"/>
+    <tableColumn id="8" name="[ABGroup]" dataDxfId="30"/>
+    <tableColumn id="4" name="[startDate]" dataDxfId="29"/>
+    <tableColumn id="5" name="[endDate]" dataDxfId="28"/>
+    <tableColumn id="10" name="[recruitingLimitDate]" dataDxfId="27"/>
+    <tableColumn id="6" name="[minRuns]" dataDxfId="26"/>
+    <tableColumn id="7" name="[cycleSize]" dataDxfId="25"/>
+    <tableColumn id="9" name="[experiment]" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2182,10 +2074,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" topLeftCell="G12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,7 +2091,7 @@
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" customWidth="1"/>
     <col min="12" max="12" width="27" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
     <col min="14" max="14" width="25.28515625" customWidth="1"/>
@@ -2234,7 +2126,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -2243,7 +2135,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
@@ -2252,7 +2144,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2266,16 +2158,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>63</v>
+        <v>22</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="H4" s="11">
         <v>3</v>
@@ -2283,27 +2175,29 @@
       <c r="I4" s="12">
         <v>5</v>
       </c>
-      <c r="J4" s="21"/>
+      <c r="J4" s="16" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2321,7 +2215,7 @@
     </row>
     <row r="12" spans="1:14" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
@@ -2330,16 +2224,16 @@
         <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>3</v>
@@ -2351,10 +2245,10 @@
         <v>14</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M12" s="9" t="s">
         <v>2</v>
@@ -2364,17 +2258,17 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C13" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="8">
         <v>1</v>
@@ -2383,36 +2277,40 @@
         <v>15</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="I13" s="6">
         <v>1</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>23</v>
+      <c r="J13" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="K13" s="8">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
+      <c r="M13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="8">
         <v>2</v>
@@ -2424,517 +2322,412 @@
         <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="N14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="8">
+        <v>20000</v>
+      </c>
+      <c r="L14" s="8"/>
+      <c r="M14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="11">
+        <v>3</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="11">
+        <v>1</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="8">
-        <v>3</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="6">
-        <v>1</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="8">
-        <v>5000</v>
-      </c>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
+      <c r="M15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="A16" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="8">
-        <v>4</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="23">
+        <v>1</v>
+      </c>
+      <c r="F16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="H16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="23">
+        <v>10000</v>
+      </c>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="B17" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="18">
+        <v>2</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="6">
         <v>5</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="J17" s="6"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="20">
+        <v>3</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="20">
+        <v>25</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+    </row>
+    <row r="19" spans="1:14" s="13" customFormat="1" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="25">
+        <v>1</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" s="6">
-        <v>1</v>
-      </c>
-      <c r="J17" s="8" t="s">
+      <c r="H19" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="25">
+        <v>1</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="25">
+        <v>1000</v>
+      </c>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="18">
+        <v>2</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="18">
+        <v>1</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="18">
+        <v>20000</v>
+      </c>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="20">
+        <v>3</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="20">
+        <v>1</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20">
+        <v>20</v>
+      </c>
+      <c r="M21" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6">
-        <v>5</v>
-      </c>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="23">
-        <v>1</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="23">
-        <v>1</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="23">
-        <v>0</v>
-      </c>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="23">
-        <v>2</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="23" t="s">
+      <c r="C22" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="23">
+        <v>1</v>
+      </c>
+      <c r="F22" s="23" t="s">
         <v>16</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="N19" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" s="23">
-        <v>3</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="23">
-        <v>1</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="K20" s="23">
-        <v>5000</v>
-      </c>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="23">
-        <v>4</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="N21" s="23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="19" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="23">
-        <v>5</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>15</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>15</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I22" s="23">
-        <v>1</v>
-      </c>
-      <c r="J22" s="23" t="s">
-        <v>37</v>
-      </c>
+        <v>15000</v>
+      </c>
+      <c r="J22" s="23"/>
       <c r="K22" s="23"/>
-      <c r="L22" s="23">
-        <v>5</v>
-      </c>
+      <c r="L22" s="23"/>
       <c r="M22" s="23"/>
       <c r="N22" s="23"/>
     </row>
     <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="14">
-        <v>1</v>
-      </c>
-      <c r="F23" s="13" t="s">
+      <c r="A23" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="18">
+        <v>2</v>
+      </c>
+      <c r="F23" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" s="18">
+        <v>5</v>
+      </c>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="20">
+        <v>3</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-    </row>
-    <row r="24" spans="1:14" s="16" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="14">
-        <v>2</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I24" s="13">
-        <v>1</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K24" s="14">
-        <v>1000</v>
-      </c>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-    </row>
-    <row r="25" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="14">
-        <v>3</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-    </row>
-    <row r="26" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="14">
-        <v>4</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I26" s="13">
-        <v>1</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K26" s="14">
-        <v>20000</v>
-      </c>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-    </row>
-    <row r="27" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="14" t="s">
+      <c r="H24" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="14">
-        <v>5</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="13">
-        <v>1</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="13">
+      <c r="I24" s="20">
         <v>20</v>
       </c>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>36</v>
-      </c>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:B22">
-    <cfRule type="duplicateValues" dxfId="1" priority="23"/>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="duplicateValues" dxfId="4" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="duplicateValues" dxfId="3" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="36" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="35" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="32" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="31" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="30" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="29" priority="10"/>
+  <conditionalFormatting sqref="B13:B18">
+    <cfRule type="duplicateValues" dxfId="0" priority="27"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Last update. Missing a value
Former-commit-id: 6695f9ec07143f390b8ab439787f54b1ea9b66cd
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -2076,8 +2076,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,7 +2173,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
almost final content for xpromo
Former-commit-id: 2a05e7731ed3588516e69919d0e8857304b1a81b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
   <si>
     <t>[sku]</t>
   </si>
@@ -86,12 +86,6 @@
     <t>[tid]</t>
   </si>
   <si>
-    <t>TID_KILLER_WHALE</t>
-  </si>
-  <si>
-    <t>TID_MEGA_TUNA</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -176,15 +170,6 @@
     <t>cycleSize: How many days player can get a reward (make sure in rewards table we have just those number of rewards defined)</t>
   </si>
   <si>
-    <t>1601510400</t>
-  </si>
-  <si>
-    <t>1604102400</t>
-  </si>
-  <si>
-    <t>1602720000</t>
-  </si>
-  <si>
     <t>group: needed only for AB test. Json for group A should set this variable ="A", and json for group B should set this variable ="B" (so client, reading this, knows in which group is each player)</t>
   </si>
   <si>
@@ -213,13 +198,43 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>cycleSize should be equal to number of rewards in a group</t>
+  </si>
+  <si>
+    <t>1609372800</t>
+  </si>
+  <si>
+    <t>1598918400</t>
+  </si>
+  <si>
+    <t>1606780800</t>
+  </si>
+  <si>
+    <t>reward_hse_hd_1b</t>
+  </si>
+  <si>
+    <t>reward_hse_hd_2b</t>
+  </si>
+  <si>
+    <t>reward_hse_hd_3b</t>
+  </si>
+  <si>
+    <t>TID_XPROMO_HAMMERHEAD</t>
+  </si>
+  <si>
+    <t>TID_XPROMO_LASER</t>
+  </si>
+  <si>
+    <t>TID_XPROMO_PYROSHARK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,8 +300,16 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +334,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -461,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -520,73 +549,42 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -603,32 +601,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -653,26 +646,18 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -700,23 +685,17 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -735,6 +714,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -744,23 +724,17 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -779,32 +753,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -823,32 +792,27 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -873,26 +837,20 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -920,23 +878,17 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -964,23 +916,73 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
         <top style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1005,26 +1007,47 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color auto="1"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1049,7 +1072,7 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1137,6 +1160,446 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1212,13 +1675,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1255,6 +1711,13 @@
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1290,468 +1753,53 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1767,42 +1815,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table52" displayName="Table52" ref="A12:N24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table52" displayName="Table52" ref="A12:N24" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A12:N24"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="{xPromoRewardsDefinitions}" dataDxfId="18"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="17"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="16"/>
-    <tableColumn id="13" name="[ABGroup]" dataDxfId="15"/>
-    <tableColumn id="4" name="[day]" dataDxfId="14"/>
-    <tableColumn id="16" name="[origin]" dataDxfId="13"/>
-    <tableColumn id="5" name="[destination]" dataDxfId="12"/>
-    <tableColumn id="6" name="[type]" dataDxfId="11"/>
-    <tableColumn id="7" name="[amount]" dataDxfId="10"/>
-    <tableColumn id="8" name="[rewardSku]" dataDxfId="9"/>
-    <tableColumn id="14" name="[altSC]" dataDxfId="8"/>
-    <tableColumn id="15" name="[altPC]" dataDxfId="7"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="6"/>
-    <tableColumn id="10" name="[tid]" dataDxfId="5"/>
+    <tableColumn id="1" name="{xPromoRewardsDefinitions}" dataDxfId="28"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="27"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="26"/>
+    <tableColumn id="13" name="[ABGroup]" dataDxfId="25"/>
+    <tableColumn id="4" name="[day]" dataDxfId="24"/>
+    <tableColumn id="16" name="[origin]" dataDxfId="23"/>
+    <tableColumn id="5" name="[destination]" dataDxfId="22"/>
+    <tableColumn id="6" name="[type]" dataDxfId="21"/>
+    <tableColumn id="7" name="[amount]" dataDxfId="20"/>
+    <tableColumn id="8" name="[rewardSku]" dataDxfId="19"/>
+    <tableColumn id="14" name="[altSC]" dataDxfId="18"/>
+    <tableColumn id="15" name="[altPC]" dataDxfId="17"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="16"/>
+    <tableColumn id="10" name="[tid]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:J4" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:J4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="A3:J4"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{xPromoSettings}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="31"/>
-    <tableColumn id="8" name="[ABGroup]" dataDxfId="30"/>
-    <tableColumn id="4" name="[startDate]" dataDxfId="29"/>
-    <tableColumn id="5" name="[endDate]" dataDxfId="28"/>
-    <tableColumn id="10" name="[recruitingLimitDate]" dataDxfId="27"/>
-    <tableColumn id="6" name="[minRuns]" dataDxfId="26"/>
-    <tableColumn id="7" name="[cycleSize]" dataDxfId="25"/>
-    <tableColumn id="9" name="[experiment]" dataDxfId="24"/>
+    <tableColumn id="1" name="{xPromoSettings}" dataDxfId="9"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="3" name="[enabled]" dataDxfId="7"/>
+    <tableColumn id="8" name="[ABGroup]" dataDxfId="6"/>
+    <tableColumn id="4" name="[startDate]" dataDxfId="5"/>
+    <tableColumn id="5" name="[endDate]" dataDxfId="4"/>
+    <tableColumn id="10" name="[recruitingLimitDate]" dataDxfId="3"/>
+    <tableColumn id="6" name="[minRuns]" dataDxfId="2"/>
+    <tableColumn id="7" name="[cycleSize]" dataDxfId="1"/>
+    <tableColumn id="9" name="[experiment]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2076,8 +2124,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,7 +2174,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -2135,7 +2183,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
@@ -2144,7 +2192,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2158,46 +2206,49 @@
         <v>1</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="H4" s="11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I4" s="12">
         <v>3</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2215,7 +2266,7 @@
     </row>
     <row r="12" spans="1:14" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
@@ -2224,16 +2275,16 @@
         <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>3</v>
@@ -2245,10 +2296,10 @@
         <v>14</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M12" s="9" t="s">
         <v>2</v>
@@ -2262,13 +2313,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="8">
         <v>1</v>
@@ -2280,23 +2331,23 @@
         <v>16</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I13" s="6">
         <v>1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="K13" s="8">
         <v>10000</v>
       </c>
       <c r="L13" s="8"/>
-      <c r="M13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>21</v>
+      <c r="M13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2304,13 +2355,13 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" s="8">
         <v>2</v>
@@ -2322,23 +2373,23 @@
         <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I14" s="6">
         <v>1</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K14" s="8">
         <v>20000</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2346,13 +2397,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C15" s="11" t="b">
         <v>1</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" s="11">
         <v>3</v>
@@ -2364,167 +2415,179 @@
         <v>16</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I15" s="11">
         <v>1</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11">
         <v>20</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>20</v>
+        <v>33</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="23">
-        <v>1</v>
-      </c>
-      <c r="F16" s="23" t="s">
+      <c r="A16" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="25">
+        <v>1</v>
+      </c>
+      <c r="F16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="23">
+      <c r="H16" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="25">
         <v>10000</v>
       </c>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="18">
+      <c r="A17" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="27">
         <v>2</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="H17" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="28">
         <v>5</v>
       </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="N17" s="27" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="20">
+      <c r="A18" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="31">
         <v>3</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" s="20">
+      <c r="H18" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="31">
         <v>25</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" s="31" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:14" s="13" customFormat="1" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="25" t="s">
+      <c r="A19" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="23">
+        <v>1</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="23">
+        <v>1</v>
+      </c>
+      <c r="J19" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="25">
-        <v>1</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I19" s="25">
-        <v>1</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="K19" s="25">
+      <c r="K19" s="23">
         <v>1000</v>
       </c>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="N19" s="25" t="s">
-        <v>62</v>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="N19" s="23" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2532,13 +2595,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="18" t="b">
         <v>1</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E20" s="18">
         <v>2</v>
@@ -2556,17 +2619,17 @@
         <v>1</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K20" s="18">
         <v>20000</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2574,13 +2637,13 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" s="20" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" s="20">
         <v>3</v>
@@ -2598,136 +2661,152 @@
         <v>1</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20">
         <v>20</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="23">
-        <v>1</v>
-      </c>
-      <c r="F22" s="23" t="s">
+      <c r="A22" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="25">
+        <v>1</v>
+      </c>
+      <c r="F22" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="23">
+      <c r="H22" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="25">
         <v>15000</v>
       </c>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="25" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="18">
+      <c r="A23" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="27">
         <v>2</v>
       </c>
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23" s="18">
-        <v>5</v>
-      </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
+      <c r="H23" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="27">
+        <v>10</v>
+      </c>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="N23" s="27" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="20">
+      <c r="A24" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="31">
         <v>3</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H24" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="I24" s="20">
-        <v>20</v>
-      </c>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
+      <c r="H24" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="31">
+        <v>1</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" s="27">
+        <v>20000</v>
+      </c>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="N24" s="31" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="4" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="3" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="2" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B18">
-    <cfRule type="duplicateValues" dxfId="0" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="27"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding tids for coins and gems rewards
Former-commit-id: 693fcba51a55f09b7bd808c9c09b342ca14cbdab
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
   <si>
     <t>[sku]</t>
   </si>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>TID_XPROMO_PYROSHARK</t>
+  </si>
+  <si>
+    <t>GR_coins_pack06</t>
+  </si>
+  <si>
+    <t>GR_gems_pack05</t>
+  </si>
+  <si>
+    <t>TID_SC_NAME_PLURAL</t>
+  </si>
+  <si>
+    <t>TID_GEM_PLURAL</t>
   </si>
 </sst>
 </file>
@@ -2124,8 +2136,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,10 +2478,10 @@
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
       <c r="M16" s="25" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2504,10 +2516,10 @@
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
       <c r="M17" s="27" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2542,10 +2554,10 @@
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
       <c r="M18" s="31" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="N18" s="31" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="13" customFormat="1" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixing Coins and Gems names
Former-commit-id: 832704b0d51320a90ad43bfe4afbcca8ac0384d8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="74">
   <si>
     <t>[sku]</t>
   </si>
@@ -95,9 +95,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>coins</t>
-  </si>
-  <si>
     <t>shark</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>dragon_reptile</t>
   </si>
   <si>
-    <t>recruitingDuration: Days when players can start the xpromo, starting from [startDate] (this is a date also)</t>
-  </si>
-  <si>
     <t>cycleSize: How many days player can get a reward (make sure in rewards table we have just those number of rewards defined)</t>
   </si>
   <si>
@@ -191,9 +185,6 @@
     <t>reward_hd_hse_3b</t>
   </si>
   <si>
-    <t>gems</t>
-  </si>
-  <si>
     <t>01-10-2020_test_x_promo_A</t>
   </si>
   <si>
@@ -240,6 +231,21 @@
   </si>
   <si>
     <t>TID_GEM_PLURAL</t>
+  </si>
+  <si>
+    <t>Coins</t>
+  </si>
+  <si>
+    <t>Gems</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>hc</t>
+  </si>
+  <si>
+    <t>recruitingLimitDuration: Days when players can start the xpromo, starting from [startDate] (this is a date also)</t>
   </si>
 </sst>
 </file>
@@ -2136,8 +2142,8 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,7 +2192,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -2195,7 +2201,7 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>10</v>
@@ -2204,7 +2210,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2221,13 +2227,13 @@
         <v>20</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H4" s="11">
         <v>7</v>
@@ -2236,25 +2242,25 @@
         <v>3</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2278,7 +2284,7 @@
     </row>
     <row r="12" spans="1:14" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>0</v>
@@ -2287,16 +2293,16 @@
         <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>3</v>
@@ -2308,10 +2314,10 @@
         <v>14</v>
       </c>
       <c r="K12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="M12" s="9" t="s">
         <v>2</v>
@@ -2325,7 +2331,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="6" t="b">
         <v>1</v>
@@ -2343,23 +2349,23 @@
         <v>16</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I13" s="6">
         <v>1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K13" s="8">
         <v>10000</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2367,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="b">
         <v>1</v>
@@ -2385,23 +2391,23 @@
         <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I14" s="6">
         <v>1</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K14" s="8">
         <v>20000</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2409,7 +2415,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="11" t="b">
         <v>1</v>
@@ -2427,23 +2433,23 @@
         <v>16</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I15" s="11">
         <v>1</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11">
         <v>20</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2451,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="25" t="b">
         <v>1</v>
@@ -2469,19 +2475,21 @@
         <v>16</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="I16" s="25">
         <v>10000</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="25" t="s">
+        <v>69</v>
+      </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
       <c r="M16" s="25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2489,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="27" t="b">
         <v>1</v>
@@ -2507,19 +2515,21 @@
         <v>16</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="I17" s="28">
         <v>5</v>
       </c>
-      <c r="J17" s="28"/>
+      <c r="J17" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
       <c r="M17" s="27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2527,7 +2537,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="31" t="b">
         <v>1</v>
@@ -2545,19 +2555,21 @@
         <v>16</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="I18" s="31">
         <v>25</v>
       </c>
-      <c r="J18" s="31"/>
+      <c r="J18" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
       <c r="M18" s="31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N18" s="31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="13" customFormat="1" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2565,7 +2577,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="23" t="b">
         <v>1</v>
@@ -2583,23 +2595,23 @@
         <v>15</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" s="23">
         <v>1</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K19" s="23">
         <v>1000</v>
       </c>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N19" s="23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2607,7 +2619,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="18" t="b">
         <v>1</v>
@@ -2631,17 +2643,17 @@
         <v>1</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K20" s="18">
         <v>20000</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2649,7 +2661,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="20" t="b">
         <v>1</v>
@@ -2673,17 +2685,17 @@
         <v>1</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20">
         <v>20</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2691,7 +2703,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C22" s="25" t="b">
         <v>1</v>
@@ -2709,19 +2721,21 @@
         <v>15</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="I22" s="25">
         <v>15000</v>
       </c>
-      <c r="J22" s="25"/>
+      <c r="J22" s="25" t="s">
+        <v>69</v>
+      </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
       <c r="M22" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2729,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C23" s="27" t="b">
         <v>1</v>
@@ -2747,19 +2761,21 @@
         <v>15</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="I23" s="27">
         <v>10</v>
       </c>
-      <c r="J23" s="27"/>
+      <c r="J23" s="27" t="s">
+        <v>70</v>
+      </c>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N23" s="27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2767,7 +2783,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C24" s="31" t="b">
         <v>1</v>
@@ -2791,17 +2807,17 @@
         <v>1</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K24" s="27">
         <v>20000</v>
       </c>
       <c r="L24" s="31"/>
       <c r="M24" s="31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting xpromo to false
Former-commit-id: dd2a6777e62671f7e589fb88729f47f54309d746
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -2143,7 +2143,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,7 +2221,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Adding missing assets (texts and some icons)
Former-commit-id: 6446cdbde9e470aa21620a21f46d108e4e077f9f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
   <si>
     <t>[sku]</t>
   </si>
@@ -188,9 +188,6 @@
     <t>01-10-2020_test_x_promo_A</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>cycleSize should be equal to number of rewards in a group</t>
   </si>
   <si>
@@ -252,6 +249,30 @@
   </si>
   <si>
     <t>icon_egg_better</t>
+  </si>
+  <si>
+    <t>icon_reptile_0</t>
+  </si>
+  <si>
+    <t>coin_visual</t>
+  </si>
+  <si>
+    <t>gem_visual</t>
+  </si>
+  <si>
+    <t>TID_XPROMO_REWARD_EGG_BETTER</t>
+  </si>
+  <si>
+    <t>TID_XPROMO_REWARD_PET_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TID_XPROMO_REWARD_DRAGON_REPTILE</t>
+  </si>
+  <si>
+    <t>FE_POPUP_IAP_COINS_LOWERCASE</t>
+  </si>
+  <si>
+    <t>FE_POPUP_IAP_GEMS_LOWERCASE</t>
   </si>
 </sst>
 </file>
@@ -2149,7 +2170,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,7 +2187,7 @@
     <col min="10" max="10" width="26.140625" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" customWidth="1"/>
+    <col min="14" max="14" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
@@ -2233,13 +2254,13 @@
         <v>20</v>
       </c>
       <c r="E4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>58</v>
       </c>
       <c r="H4" s="11">
         <v>7</v>
@@ -2258,7 +2279,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2266,7 +2287,7 @@
         <v>45</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2371,7 +2392,7 @@
         <v>33</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2413,7 +2434,7 @@
         <v>49</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2455,7 +2476,7 @@
         <v>32</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2481,21 +2502,21 @@
         <v>16</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I16" s="25">
         <v>10000</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
       <c r="M16" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -2521,21 +2542,21 @@
         <v>16</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I17" s="28">
         <v>5</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
       <c r="M17" s="27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2561,21 +2582,21 @@
         <v>16</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I18" s="31">
         <v>25</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
       <c r="M18" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N18" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="13" customFormat="1" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2614,10 +2635,10 @@
       </c>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N19" s="23" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2656,10 +2677,10 @@
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2698,10 +2719,10 @@
         <v>20</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2709,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="25" t="b">
         <v>1</v>
@@ -2727,21 +2748,21 @@
         <v>15</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I22" s="25">
         <v>15000</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
       <c r="M22" s="25" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2749,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="27" t="b">
         <v>1</v>
@@ -2767,21 +2788,21 @@
         <v>15</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I23" s="27">
         <v>10</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="N23" s="27" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2789,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="31" t="b">
         <v>1</v>
@@ -2820,10 +2841,10 @@
       </c>
       <c r="L24" s="31"/>
       <c r="M24" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XPromo - Fix content: wrong reward for HSE
Former-commit-id: 774ea2d4ad578cc6448d9d9fcb79f588e10b4ac6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Xpromo.xlsx
+++ b/Docs/Content/HungryDragonContent_Xpromo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76B281E-BACB-AD4C-9C3B-3A57BC0FB03F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19200" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26000" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Special Leagues" sheetId="16" r:id="rId1"/>
@@ -122,9 +123,6 @@
     <t>egg</t>
   </si>
   <si>
-    <t>SD_shark_moby</t>
-  </si>
-  <si>
     <t>SD_shark_hammerhead</t>
   </si>
   <si>
@@ -176,9 +174,6 @@
     <t>Laser</t>
   </si>
   <si>
-    <t>moby</t>
-  </si>
-  <si>
     <t>reward_hd_hse_3a</t>
   </si>
   <si>
@@ -273,12 +268,18 @@
   </si>
   <si>
     <t>FE_POPUP_IAP_GEMS_LOWERCASE</t>
+  </si>
+  <si>
+    <t>SD_shark_pyro</t>
+  </si>
+  <si>
+    <t>pyro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1860,42 +1861,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table52" displayName="Table52" ref="A12:N24" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
-  <autoFilter ref="A12:N24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table52" displayName="Table52" ref="A12:N24" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+  <autoFilter ref="A12:N24" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="{xPromoRewardsDefinitions}" dataDxfId="28"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="27"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="26"/>
-    <tableColumn id="13" name="[ABGroup]" dataDxfId="25"/>
-    <tableColumn id="4" name="[day]" dataDxfId="24"/>
-    <tableColumn id="16" name="[origin]" dataDxfId="23"/>
-    <tableColumn id="5" name="[destination]" dataDxfId="22"/>
-    <tableColumn id="6" name="[type]" dataDxfId="21"/>
-    <tableColumn id="7" name="[amount]" dataDxfId="20"/>
-    <tableColumn id="8" name="[rewardSku]" dataDxfId="19"/>
-    <tableColumn id="14" name="[altSC]" dataDxfId="18"/>
-    <tableColumn id="15" name="[altPC]" dataDxfId="17"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="16"/>
-    <tableColumn id="10" name="[tid]" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{xPromoRewardsDefinitions}" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enabled]" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[ABGroup]" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[day]" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[origin]" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[destination]" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[type]" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[amount]" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[rewardSku]" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[altSC]" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[altPC]" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[icon]" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[tid]" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:J4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A3:J4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A3:J4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A3:J4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="{xPromoSettings}" dataDxfId="9"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="8"/>
-    <tableColumn id="3" name="[enabled]" dataDxfId="7"/>
-    <tableColumn id="8" name="[ABGroup]" dataDxfId="6"/>
-    <tableColumn id="4" name="[startDate]" dataDxfId="5"/>
-    <tableColumn id="5" name="[endDate]" dataDxfId="4"/>
-    <tableColumn id="10" name="[recruitingLimitDate]" dataDxfId="3"/>
-    <tableColumn id="6" name="[minRuns]" dataDxfId="2"/>
-    <tableColumn id="7" name="[cycleSize]" dataDxfId="1"/>
-    <tableColumn id="9" name="[experiment]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{xPromoSettings}" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[enabled]" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="[ABGroup]" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="[startDate]" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="[endDate]" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="[recruitingLimitDate]" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="[minRuns]" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[cycleSize]" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="[experiment]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2163,34 +2164,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="G10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
     <col min="13" max="13" width="23" customWidth="1"/>
-    <col min="14" max="14" width="38.42578125" customWidth="1"/>
+    <col min="14" max="14" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2202,13 +2203,13 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:14" ht="105.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="103" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2237,10 +2238,10 @@
         <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
@@ -2254,13 +2255,13 @@
         <v>20</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>55</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>57</v>
       </c>
       <c r="H4" s="11">
         <v>7</v>
@@ -2269,29 +2270,29 @@
         <v>3</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:14" ht="24" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -2303,13 +2304,13 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:14" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="137" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -2353,12 +2354,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="6" t="b">
         <v>1</v>
@@ -2382,25 +2383,25 @@
         <v>1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K13" s="8">
         <v>10000</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="6" t="b">
         <v>1</v>
@@ -2418,31 +2419,31 @@
         <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="I14" s="6">
-        <v>1</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="K14" s="8">
         <v>20000</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="C15" s="11" t="b">
         <v>1</v>
@@ -2466,25 +2467,25 @@
         <v>1</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11">
         <v>20</v>
       </c>
-      <c r="M15" s="8" t="s">
-        <v>32</v>
+      <c r="M15" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="25" t="b">
         <v>1</v>
@@ -2502,29 +2503,29 @@
         <v>16</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I16" s="25">
         <v>10000</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
       <c r="M16" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="25" t="s">
-        <v>66</v>
-      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="27" t="b">
         <v>1</v>
@@ -2542,29 +2543,29 @@
         <v>16</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I17" s="28">
         <v>5</v>
       </c>
       <c r="J17" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
       <c r="M17" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="N17" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="N17" s="27" t="s">
-        <v>67</v>
-      </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="31" t="b">
         <v>1</v>
@@ -2582,29 +2583,29 @@
         <v>16</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I18" s="31">
         <v>25</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
       <c r="M18" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="N18" s="31" t="s">
-        <v>67</v>
-      </c>
     </row>
-    <row r="19" spans="1:14" s="13" customFormat="1" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="13" customFormat="1" ht="16" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="23" t="b">
         <v>1</v>
@@ -2628,25 +2629,25 @@
         <v>1</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K19" s="23">
         <v>1000</v>
       </c>
       <c r="L19" s="23"/>
       <c r="M19" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N19" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="18" t="b">
         <v>1</v>
@@ -2670,25 +2671,25 @@
         <v>1</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K20" s="18">
         <v>20000</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="20" t="b">
         <v>1</v>
@@ -2712,25 +2713,25 @@
         <v>1</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20">
         <v>20</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="25" t="b">
         <v>1</v>
@@ -2748,29 +2749,29 @@
         <v>15</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I22" s="25">
         <v>15000</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K22" s="25"/>
       <c r="L22" s="25"/>
       <c r="M22" s="25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" s="27" t="b">
         <v>1</v>
@@ -2788,29 +2789,29 @@
         <v>15</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I23" s="27">
         <v>10</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K23" s="27"/>
       <c r="L23" s="27"/>
       <c r="M23" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="N23" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" s="31" t="b">
         <v>1</v>
@@ -2834,17 +2835,17 @@
         <v>1</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K24" s="27">
         <v>20000</v>
       </c>
       <c r="L24" s="31"/>
       <c r="M24" s="31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N24" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>